<commit_message>
Tidsregistrering Allan - samt billede af rettelser vil vores program.
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Allan Strange - Tidsregistrering.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Allan Strange - Tidsregistrering.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="93">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -298,6 +298,18 @@
   </si>
   <si>
     <t>Implementeret test til Test Suite OC7</t>
+  </si>
+  <si>
+    <t>Implementeret ReferencespaendingTest</t>
+  </si>
+  <si>
+    <t>Aflevering af projektet</t>
+  </si>
+  <si>
+    <t>Undervisning</t>
+  </si>
+  <si>
+    <t>sigmaRef regner forkert</t>
   </si>
 </sst>
 </file>
@@ -401,8 +413,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A3:I30" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A3:I30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A3:I34" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A3:I34"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Kolonne1" dataDxfId="2"/>
     <tableColumn id="2" name="Kolonne2"/>
@@ -715,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,6 +1420,98 @@
       </c>
       <c r="I30" s="5">
         <v>0.11458333333333333</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31" t="s">
+        <v>89</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H31" s="5">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="I31" s="5">
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" t="s">
+        <v>90</v>
+      </c>
+      <c r="G32" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="H32" s="5">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="I32" s="5">
+        <v>4.8611111111111112E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" t="s">
+        <v>56</v>
+      </c>
+      <c r="F33" t="s">
+        <v>91</v>
+      </c>
+      <c r="G33" s="5">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="H33" s="5">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="I33" s="5">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>42817</v>
+      </c>
+      <c r="B34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" t="s">
+        <v>56</v>
+      </c>
+      <c r="F34" t="s">
+        <v>92</v>
+      </c>
+      <c r="G34" s="5">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="H34" s="5">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="I34" s="5">
+        <v>6.25E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>